<commit_message>
Graphs completed. Submission almost ready.
</commit_message>
<xml_diff>
--- a/Graphs/diabetes_knn.xlsx
+++ b/Graphs/diabetes_knn.xlsx
@@ -17,6 +17,18 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$B$14:$B$18</definedName>
+    <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$C$13</definedName>
+    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$C$14:$C$18</definedName>
+    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$D$13</definedName>
+    <definedName name="_xlchart.v3.4" hidden="1">Sheet1!$D$14:$D$18</definedName>
+    <definedName name="_xlchart.v3.5" hidden="1">Sheet1!$E$13</definedName>
+    <definedName name="_xlchart.v3.6" hidden="1">Sheet1!$E$14:$E$18</definedName>
+    <definedName name="_xlchart.v3.7" hidden="1">Sheet1!$F$13</definedName>
+    <definedName name="_xlchart.v3.8" hidden="1">Sheet1!$F$14:$F$18</definedName>
+    <definedName name="_xlchart.v3.9" hidden="1">Sheet1!$F$14:$F$18</definedName>
+  </definedNames>
   <calcPr calcId="171027" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -190,12 +202,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Diabetes K-NN Train/Test Accuracy</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1600">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -234,7 +246,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -754,7 +766,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1874,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>